<commit_message>
more mde concepts agentur fine concepts
</commit_message>
<xml_diff>
--- a/zeitgeist/concepts/agentur/agentur_spielfeld.xlsx
+++ b/zeitgeist/concepts/agentur/agentur_spielfeld.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Eregniskarten" sheetId="2" r:id="rId2"/>
     <sheet name="Mitarbeiterkarten" sheetId="3" r:id="rId3"/>
     <sheet name="Projekkarten" sheetId="4" r:id="rId4"/>
+    <sheet name="Learnings" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="81">
   <si>
     <t>Start</t>
   </si>
@@ -184,13 +185,7 @@
     <t>Strategie &amp; Konzept</t>
   </si>
   <si>
-    <t>Punkt</t>
-  </si>
-  <si>
     <t>Die Bank zahlt Dir eine Dividende</t>
-  </si>
-  <si>
-    <t>In einem Artikel ist deine Agentur ganz vorne mit dabei</t>
   </si>
   <si>
     <t>Ziehe 2 Felder vor</t>
@@ -235,13 +230,55 @@
 Kreation &amp; Design
 Umsetzung &amp; Technik
 Service &amp; Betreuung</t>
+  </si>
+  <si>
+    <t>Geld</t>
+  </si>
+  <si>
+    <t>Visitenkarten</t>
+  </si>
+  <si>
+    <t>Würfel</t>
+  </si>
+  <si>
+    <t>in Projekt</t>
+  </si>
+  <si>
+    <t>Projekte</t>
+  </si>
+  <si>
+    <t>Mitarbeitertyp</t>
+  </si>
+  <si>
+    <t>Umsetzung</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Ablösesumme</t>
+  </si>
+  <si>
+    <t>Punkte</t>
+  </si>
+  <si>
+    <t>Das Weihnachtsgeld steht an</t>
+  </si>
+  <si>
+    <t>Zahle für jeden deiner Mitarbeiter 1000 Euro in den Pool</t>
+  </si>
+  <si>
+    <t>In einem Zeitungsartikel ist deine Agentur ganz vorne mit dabei</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +289,42 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -427,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -463,6 +536,35 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -757,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L12"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -768,81 +870,129 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="12" customWidth="1"/>
     <col min="4" max="12" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:23">
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+    </row>
+    <row r="3" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" s="12" customFormat="1" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B3" s="13" t="s">
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="30"/>
+      <c r="P3" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="41">
+        <f ca="1">RANDBETWEEN(1,12)</f>
+        <v>3</v>
+      </c>
+      <c r="R3" s="31">
+        <f ca="1">RANDBETWEEN(0,10)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="12" customFormat="1" ht="50.1" customHeight="1" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="13" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B4" s="28" t="s">
+      <c r="M4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B5" s="28" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B5" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="18"/>
@@ -853,13 +1003,19 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="19"/>
-      <c r="L5" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B6" s="13" t="s">
+      <c r="L5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="29">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="18"/>
@@ -873,42 +1029,63 @@
       <c r="L6" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B7" s="3" t="s">
+      <c r="P6" s="33"/>
+      <c r="Q6" s="29"/>
+    </row>
+    <row r="7" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+    </row>
+    <row r="8" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="3" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="40"/>
+    </row>
+    <row r="9" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
@@ -921,13 +1098,24 @@
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="19"/>
-      <c r="L9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B10" s="1" t="s">
-        <v>5</v>
+      <c r="L9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="40"/>
+    </row>
+    <row r="10" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B10" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -938,59 +1126,210 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="19"/>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q10" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="R10" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="V10" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="W10" s="34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B11" s="13" t="s">
+      <c r="O11" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="39">
+        <v>2</v>
+      </c>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39">
+        <v>2000</v>
+      </c>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="40"/>
+    </row>
+    <row r="12" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="13" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B12" s="2" t="s">
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q12" s="39">
+        <v>2</v>
+      </c>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39">
+        <v>2000</v>
+      </c>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="40"/>
+    </row>
+    <row r="13" spans="1:23" ht="50.1" customHeight="1" thickBot="1">
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="28" t="s">
+      <c r="C13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L13" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="N13" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="39">
+        <v>1</v>
+      </c>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39">
+        <v>1000</v>
+      </c>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="40"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="36">
+        <v>1</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36">
+        <v>1</v>
+      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="38"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="38"/>
+      <c r="V16" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1000,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1013,15 +1352,19 @@
     <col min="3" max="3" width="69.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:5" ht="31.5">
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="E2" s="30">
+        <f ca="1">RANDBETWEEN(2,21)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -1029,55 +1372,73 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:5">
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="2:3">
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:3">
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="2:3">
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="2:3">
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1085,7 +1446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:5">
       <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
@@ -1093,7 +1454,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:5">
       <c r="B12" s="6" t="s">
         <v>32</v>
       </c>
@@ -1101,7 +1462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:5">
       <c r="B13" s="6" t="s">
         <v>26</v>
       </c>
@@ -1109,7 +1470,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:5">
       <c r="B14" s="6" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:5">
       <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
@@ -1125,7 +1486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:5">
       <c r="B16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1151,7 +1512,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>18</v>
@@ -1159,10 +1520,18 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="7" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1172,18 +1541,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E30"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="4" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" ht="31.5">
       <c r="A2" s="8" t="s">
         <v>45</v>
       </c>
@@ -1194,13 +1566,20 @@
         <v>44</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="30">
+        <f ca="1">RANDBETWEEN(3,18)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>49</v>
       </c>
@@ -1214,110 +1593,134 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
+        <v>2500</v>
+      </c>
+      <c r="F4">
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5">
+        <v>5000</v>
+      </c>
+      <c r="F5">
         <v>2000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
       </c>
       <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>7500</v>
+      </c>
+      <c r="F6">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" t="s">
+      <c r="E8">
+        <v>2500</v>
+      </c>
+      <c r="F8">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7">
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9">
         <v>4</v>
-      </c>
-      <c r="E7">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
       </c>
       <c r="E9">
         <v>5000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>7500</v>
+      </c>
+      <c r="F10">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1326,270 +1729,120 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12">
+        <v>2500</v>
+      </c>
+      <c r="F12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>5000</v>
+      </c>
+      <c r="F13">
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
+    <row r="14" spans="1:7">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>7500</v>
+      </c>
+      <c r="F14">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13">
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="E16">
+        <v>2500</v>
+      </c>
+      <c r="F16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>5000</v>
+      </c>
+      <c r="F17">
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
-      </c>
-      <c r="E22">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23">
-        <v>8</v>
-      </c>
-      <c r="E23">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-      <c r="E28">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-      <c r="E29">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30">
-        <v>8</v>
-      </c>
-      <c r="E30">
-        <v>5000</v>
+        <v>7500</v>
+      </c>
+      <c r="F18">
+        <v>3500</v>
       </c>
     </row>
   </sheetData>
@@ -1600,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1612,18 +1865,18 @@
     <col min="2" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
         <v>51</v>
       </c>
@@ -1634,7 +1887,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" s="9" t="s">
         <v>52</v>
       </c>
@@ -1645,7 +1898,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
@@ -1656,7 +1909,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
         <v>54</v>
       </c>
@@ -1667,96 +1920,120 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="9">
         <v>2</v>
       </c>
       <c r="C7" s="9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30">
+        <v>4000</v>
+      </c>
+      <c r="F7" s="30">
+        <f ca="1">RANDBETWEEN(3,14)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="9">
         <v>2</v>
       </c>
       <c r="C8" s="9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30">
+        <v>4000</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="9">
         <v>2</v>
       </c>
       <c r="C9" s="9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30">
+        <v>4000</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="9">
         <v>2</v>
       </c>
       <c r="C10" s="9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="9">
         <v>3</v>
       </c>
       <c r="C11" s="9">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="9">
         <v>3</v>
       </c>
       <c r="C12" s="9">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="60">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60">
       <c r="A13" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="9">
         <v>4</v>
       </c>
       <c r="C13" s="9">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="60">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60">
       <c r="A14" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" s="9">
         <v>4</v>
       </c>
       <c r="C14" s="9">
-        <v>15000</v>
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>